<commit_message>
fixing scenaries plot bug, and exporting scenario profits projections
</commit_message>
<xml_diff>
--- a/data/ganancias.xlsx
+++ b/data/ganancias.xlsx
@@ -7,16 +7,28 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Goldwind GW87 1500" sheetId="1" r:id="rId1"/>
-    <sheet name="Vestas V110 2000" sheetId="2" r:id="rId2"/>
-    <sheet name="Vestas V100 2000" sheetId="3" r:id="rId3"/>
+    <sheet name="Goldwind GW87 1500-escenario_a" sheetId="1" r:id="rId1"/>
+    <sheet name="Goldwind GW87 1500-escenario_b" sheetId="2" r:id="rId2"/>
+    <sheet name="Goldwind GW87 1500-escenario_c" sheetId="3" r:id="rId3"/>
+    <sheet name="Goldwind GW87 1500-escenario_d" sheetId="4" r:id="rId4"/>
+    <sheet name="Goldwind GW87 1500-escenario_e" sheetId="5" r:id="rId5"/>
+    <sheet name="Vestas V110 2000-escenario_a" sheetId="6" r:id="rId6"/>
+    <sheet name="Vestas V110 2000-escenario_b" sheetId="7" r:id="rId7"/>
+    <sheet name="Vestas V110 2000-escenario_c" sheetId="8" r:id="rId8"/>
+    <sheet name="Vestas V110 2000-escenario_d" sheetId="9" r:id="rId9"/>
+    <sheet name="Vestas V110 2000-escenario_e" sheetId="10" r:id="rId10"/>
+    <sheet name="Vestas V100 2000-escenario_a" sheetId="11" r:id="rId11"/>
+    <sheet name="Vestas V100 2000-escenario_b" sheetId="12" r:id="rId12"/>
+    <sheet name="Vestas V100 2000-escenario_c" sheetId="13" r:id="rId13"/>
+    <sheet name="Vestas V100 2000-escenario_d" sheetId="14" r:id="rId14"/>
+    <sheet name="Vestas V100 2000-escenario_e" sheetId="15" r:id="rId15"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="2">
   <si>
     <t>year</t>
   </si>
@@ -558,6 +570,1092 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>2024</v>
+      </c>
+      <c r="B2">
+        <v>5161409.676904143</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>2025</v>
+      </c>
+      <c r="B3">
+        <v>5090736.111486748</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>2026</v>
+      </c>
+      <c r="B4">
+        <v>5944472.67064536</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>2027</v>
+      </c>
+      <c r="B5">
+        <v>6485535.767885554</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>2028</v>
+      </c>
+      <c r="B6">
+        <v>6682918.274372596</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>2029</v>
+      </c>
+      <c r="B7">
+        <v>6904841.061887729</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>2030</v>
+      </c>
+      <c r="B8">
+        <v>6592261.460922168</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <v>2031</v>
+      </c>
+      <c r="B9">
+        <v>6029002.137555054</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>2032</v>
+      </c>
+      <c r="B10">
+        <v>5879271.864519663</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11">
+        <v>2033</v>
+      </c>
+      <c r="B11">
+        <v>5980204.044909685</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12">
+        <v>2034</v>
+      </c>
+      <c r="B12">
+        <v>5208952.195745756</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13">
+        <v>2035</v>
+      </c>
+      <c r="B13">
+        <v>4559919.104986785</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14">
+        <v>2036</v>
+      </c>
+      <c r="B14">
+        <v>4888444.974029092</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15">
+        <v>2037</v>
+      </c>
+      <c r="B15">
+        <v>4247105.788151414</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16">
+        <v>2038</v>
+      </c>
+      <c r="B16">
+        <v>4261743.552037084</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17">
+        <v>2039</v>
+      </c>
+      <c r="B17">
+        <v>4688163.134689402</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18">
+        <v>2040</v>
+      </c>
+      <c r="B18">
+        <v>4639685.068129502</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19">
+        <v>2041</v>
+      </c>
+      <c r="B19">
+        <v>5265969.56493327</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20">
+        <v>2042</v>
+      </c>
+      <c r="B20">
+        <v>5344394.918972166</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21">
+        <v>2043</v>
+      </c>
+      <c r="B21">
+        <v>5591412.284688175</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>2024</v>
+      </c>
+      <c r="B2">
+        <v>7769536.620339863</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>2025</v>
+      </c>
+      <c r="B3">
+        <v>6513521.261481231</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>2026</v>
+      </c>
+      <c r="B4">
+        <v>7685606.660136452</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>2027</v>
+      </c>
+      <c r="B5">
+        <v>8375048.839184897</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>2028</v>
+      </c>
+      <c r="B6">
+        <v>8441419.524338195</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>2029</v>
+      </c>
+      <c r="B7">
+        <v>8710851.573803432</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>2030</v>
+      </c>
+      <c r="B8">
+        <v>8496392.817765646</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <v>2031</v>
+      </c>
+      <c r="B9">
+        <v>9056455.227835827</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>2032</v>
+      </c>
+      <c r="B10">
+        <v>9255619.398572583</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11">
+        <v>2033</v>
+      </c>
+      <c r="B11">
+        <v>9904333.984707642</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12">
+        <v>2034</v>
+      </c>
+      <c r="B12">
+        <v>8840679.935987633</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13">
+        <v>2035</v>
+      </c>
+      <c r="B13">
+        <v>9388959.156573191</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14">
+        <v>2036</v>
+      </c>
+      <c r="B14">
+        <v>10083511.84565322</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15">
+        <v>2037</v>
+      </c>
+      <c r="B15">
+        <v>8980054.468417412</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16">
+        <v>2038</v>
+      </c>
+      <c r="B16">
+        <v>9808145.172027892</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17">
+        <v>2039</v>
+      </c>
+      <c r="B17">
+        <v>10832623.48181518</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18">
+        <v>2040</v>
+      </c>
+      <c r="B18">
+        <v>11351116.19753434</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19">
+        <v>2041</v>
+      </c>
+      <c r="B19">
+        <v>11569728.63170497</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20">
+        <v>2042</v>
+      </c>
+      <c r="B20">
+        <v>12026256.87803554</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21">
+        <v>2043</v>
+      </c>
+      <c r="B21">
+        <v>12390830.27578433</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>2024</v>
+      </c>
+      <c r="B2">
+        <v>4795967.926296496</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>2025</v>
+      </c>
+      <c r="B3">
+        <v>4870014.96509698</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>2026</v>
+      </c>
+      <c r="B4">
+        <v>5752495.630876959</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>2027</v>
+      </c>
+      <c r="B5">
+        <v>6252555.119209604</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>2028</v>
+      </c>
+      <c r="B6">
+        <v>6422901.974170445</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>2029</v>
+      </c>
+      <c r="B7">
+        <v>6847440.095773663</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>2030</v>
+      </c>
+      <c r="B8">
+        <v>6672465.485246865</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <v>2031</v>
+      </c>
+      <c r="B9">
+        <v>6775116.537790397</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>2032</v>
+      </c>
+      <c r="B10">
+        <v>6856795.287017842</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11">
+        <v>2033</v>
+      </c>
+      <c r="B11">
+        <v>7057618.732947132</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12">
+        <v>2034</v>
+      </c>
+      <c r="B12">
+        <v>6870014.219242302</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13">
+        <v>2035</v>
+      </c>
+      <c r="B13">
+        <v>6354298.285231301</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14">
+        <v>2036</v>
+      </c>
+      <c r="B14">
+        <v>6688761.603619129</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15">
+        <v>2037</v>
+      </c>
+      <c r="B15">
+        <v>6433470.281059078</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16">
+        <v>2038</v>
+      </c>
+      <c r="B16">
+        <v>7078803.56654714</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17">
+        <v>2039</v>
+      </c>
+      <c r="B17">
+        <v>7853746.054595947</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18">
+        <v>2040</v>
+      </c>
+      <c r="B18">
+        <v>8349559.047455871</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19">
+        <v>2041</v>
+      </c>
+      <c r="B19">
+        <v>8513672.961064409</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20">
+        <v>2042</v>
+      </c>
+      <c r="B20">
+        <v>8638532.187419623</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21">
+        <v>2043</v>
+      </c>
+      <c r="B21">
+        <v>8885534.905364383</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>2024</v>
+      </c>
+      <c r="B2">
+        <v>5322814.210255641</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>2025</v>
+      </c>
+      <c r="B3">
+        <v>5511008.95924887</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>2026</v>
+      </c>
+      <c r="B4">
+        <v>6478723.023322714</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>2027</v>
+      </c>
+      <c r="B5">
+        <v>6898724.342148143</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>2028</v>
+      </c>
+      <c r="B6">
+        <v>6850244.554232828</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>2029</v>
+      </c>
+      <c r="B7">
+        <v>7500165.765047994</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>2030</v>
+      </c>
+      <c r="B8">
+        <v>6840632.077799634</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <v>2031</v>
+      </c>
+      <c r="B9">
+        <v>6587619.189267986</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>2032</v>
+      </c>
+      <c r="B10">
+        <v>6492566.737051401</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11">
+        <v>2033</v>
+      </c>
+      <c r="B11">
+        <v>6575087.167506526</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12">
+        <v>2034</v>
+      </c>
+      <c r="B12">
+        <v>6152094.086737183</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13">
+        <v>2035</v>
+      </c>
+      <c r="B13">
+        <v>6090907.094043063</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14">
+        <v>2036</v>
+      </c>
+      <c r="B14">
+        <v>6548719.047785557</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15">
+        <v>2037</v>
+      </c>
+      <c r="B15">
+        <v>4558315.106154352</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16">
+        <v>2038</v>
+      </c>
+      <c r="B16">
+        <v>4943990.793853116</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17">
+        <v>2039</v>
+      </c>
+      <c r="B17">
+        <v>5415142.166384201</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18">
+        <v>2040</v>
+      </c>
+      <c r="B18">
+        <v>5089057.893352281</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19">
+        <v>2041</v>
+      </c>
+      <c r="B19">
+        <v>5682319.270964641</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20">
+        <v>2042</v>
+      </c>
+      <c r="B20">
+        <v>5997647.520150635</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21">
+        <v>2043</v>
+      </c>
+      <c r="B21">
+        <v>5974277.893817212</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>2024</v>
+      </c>
+      <c r="B2">
+        <v>9043499.73626123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>2025</v>
+      </c>
+      <c r="B3">
+        <v>7640210.949613268</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>2026</v>
+      </c>
+      <c r="B4">
+        <v>9262528.211770331</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>2027</v>
+      </c>
+      <c r="B5">
+        <v>9268775.606076684</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>2028</v>
+      </c>
+      <c r="B6">
+        <v>9285547.877199419</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>2029</v>
+      </c>
+      <c r="B7">
+        <v>8765685.927396072</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>2030</v>
+      </c>
+      <c r="B8">
+        <v>6949133.203191817</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <v>2031</v>
+      </c>
+      <c r="B9">
+        <v>6869902.173951946</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>2032</v>
+      </c>
+      <c r="B10">
+        <v>6785038.071021894</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11">
+        <v>2033</v>
+      </c>
+      <c r="B11">
+        <v>7450923.004504105</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12">
+        <v>2034</v>
+      </c>
+      <c r="B12">
+        <v>6268650.836400864</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13">
+        <v>2035</v>
+      </c>
+      <c r="B13">
+        <v>5753059.270332804</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14">
+        <v>2036</v>
+      </c>
+      <c r="B14">
+        <v>6335548.553953072</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15">
+        <v>2037</v>
+      </c>
+      <c r="B15">
+        <v>5710477.253226763</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16">
+        <v>2038</v>
+      </c>
+      <c r="B16">
+        <v>6476559.319694991</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17">
+        <v>2039</v>
+      </c>
+      <c r="B17">
+        <v>7128050.839811744</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18">
+        <v>2040</v>
+      </c>
+      <c r="B18">
+        <v>7480016.426703026</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19">
+        <v>2041</v>
+      </c>
+      <c r="B19">
+        <v>7916799.475816598</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20">
+        <v>2042</v>
+      </c>
+      <c r="B20">
+        <v>8610893.173072858</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21">
+        <v>2043</v>
+      </c>
+      <c r="B21">
+        <v>8990983.220574996</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>2024</v>
+      </c>
+      <c r="B2">
+        <v>5340462.840870301</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>2025</v>
+      </c>
+      <c r="B3">
+        <v>5267480.546903757</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>2026</v>
+      </c>
+      <c r="B4">
+        <v>6149777.888658804</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>2027</v>
+      </c>
+      <c r="B5">
+        <v>6700665.904020675</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>2028</v>
+      </c>
+      <c r="B6">
+        <v>6913120.98119905</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>2029</v>
+      </c>
+      <c r="B7">
+        <v>7155264.046978963</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>2030</v>
+      </c>
+      <c r="B8">
+        <v>6824117.851041973</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <v>2031</v>
+      </c>
+      <c r="B9">
+        <v>6228836.162864366</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>2032</v>
+      </c>
+      <c r="B10">
+        <v>6073896.256659665</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11">
+        <v>2033</v>
+      </c>
+      <c r="B11">
+        <v>6176296.231610263</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12">
+        <v>2034</v>
+      </c>
+      <c r="B12">
+        <v>5380692.517271817</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13">
+        <v>2035</v>
+      </c>
+      <c r="B13">
+        <v>4702653.180485429</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14">
+        <v>2036</v>
+      </c>
+      <c r="B14">
+        <v>5047546.955490618</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15">
+        <v>2037</v>
+      </c>
+      <c r="B15">
+        <v>4390433.91830395</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16">
+        <v>2038</v>
+      </c>
+      <c r="B16">
+        <v>4405935.090951866</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17">
+        <v>2039</v>
+      </c>
+      <c r="B17">
+        <v>4854287.364302333</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18">
+        <v>2040</v>
+      </c>
+      <c r="B18">
+        <v>4803791.740610108</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19">
+        <v>2041</v>
+      </c>
+      <c r="B19">
+        <v>5452323.492847281</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20">
+        <v>2042</v>
+      </c>
+      <c r="B20">
+        <v>5529297.527836195</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21">
+        <v>2043</v>
+      </c>
+      <c r="B21">
+        <v>5789732.371948994</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B21"/>
@@ -579,7 +1677,7 @@
         <v>2024</v>
       </c>
       <c r="B2">
-        <v>7499026.829941634</v>
+        <v>3554422.482616894</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -587,7 +1685,7 @@
         <v>2025</v>
       </c>
       <c r="B3">
-        <v>6282243.878390167</v>
+        <v>3609900.103701606</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -595,7 +1693,7 @@
         <v>2026</v>
       </c>
       <c r="B4">
-        <v>7413402.299742431</v>
+        <v>4263567.684402155</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -603,7 +1701,7 @@
         <v>2027</v>
       </c>
       <c r="B5">
-        <v>8078012.344860101</v>
+        <v>4638241.710210156</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -611,7 +1709,7 @@
         <v>2028</v>
       </c>
       <c r="B6">
-        <v>8152425.86897608</v>
+        <v>4761755.190028585</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -619,7 +1717,7 @@
         <v>2029</v>
       </c>
       <c r="B7">
-        <v>8400661.871458042</v>
+        <v>5059966.216703316</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -627,7 +1725,7 @@
         <v>2030</v>
       </c>
       <c r="B8">
-        <v>8207821.343610279</v>
+        <v>4930703.646720028</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -635,7 +1733,7 @@
         <v>2031</v>
       </c>
       <c r="B9">
-        <v>8751324.446800245</v>
+        <v>5008794.763142521</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -643,7 +1741,7 @@
         <v>2032</v>
       </c>
       <c r="B10">
-        <v>8939568.85699724</v>
+        <v>5067893.530619124</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -651,7 +1749,7 @@
         <v>2033</v>
       </c>
       <c r="B11">
-        <v>9567627.857173232</v>
+        <v>5217061.228925681</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -659,7 +1757,7 @@
         <v>2034</v>
       </c>
       <c r="B12">
-        <v>8543549.69235404</v>
+        <v>5073150.809135647</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -667,7 +1765,7 @@
         <v>2035</v>
       </c>
       <c r="B13">
-        <v>9070246.894371806</v>
+        <v>4682991.366864385</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -675,7 +1773,7 @@
         <v>2036</v>
       </c>
       <c r="B14">
-        <v>9735464.336171718</v>
+        <v>4931935.931850261</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -683,7 +1781,7 @@
         <v>2037</v>
       </c>
       <c r="B15">
-        <v>8672967.028321913</v>
+        <v>4741218.430577287</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -691,7 +1789,7 @@
         <v>2038</v>
       </c>
       <c r="B16">
-        <v>9467767.032271439</v>
+        <v>5220330.442827605</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -699,7 +1797,7 @@
         <v>2039</v>
       </c>
       <c r="B17">
-        <v>10450475.12074826</v>
+        <v>5796421.398617131</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -707,7 +1805,7 @@
         <v>2040</v>
       </c>
       <c r="B18">
-        <v>10946648.87480488</v>
+        <v>6166039.478266618</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -715,7 +1813,7 @@
         <v>2041</v>
       </c>
       <c r="B19">
-        <v>11158353.21086289</v>
+        <v>6289337.325319171</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -723,7 +1821,7 @@
         <v>2042</v>
       </c>
       <c r="B20">
-        <v>11599259.03731799</v>
+        <v>6384022.181144047</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -731,7 +1829,7 @@
         <v>2043</v>
       </c>
       <c r="B21">
-        <v>11948646.3913637</v>
+        <v>6573598.510826107</v>
       </c>
     </row>
   </sheetData>
@@ -760,7 +1858,7 @@
         <v>2024</v>
       </c>
       <c r="B2">
-        <v>7769536.620339863</v>
+        <v>3940149.740024171</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -768,7 +1866,7 @@
         <v>2025</v>
       </c>
       <c r="B3">
-        <v>6513521.261481231</v>
+        <v>4078515.266303315</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -776,7 +1874,7 @@
         <v>2026</v>
       </c>
       <c r="B4">
-        <v>7685606.660136452</v>
+        <v>4793078.278074741</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -784,7 +1882,7 @@
         <v>2027</v>
       </c>
       <c r="B5">
-        <v>8375048.839184897</v>
+        <v>5104167.446943546</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -792,7 +1890,7 @@
         <v>2028</v>
       </c>
       <c r="B6">
-        <v>8441419.524338195</v>
+        <v>5064718.708534096</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -800,7 +1898,7 @@
         <v>2029</v>
       </c>
       <c r="B7">
-        <v>8710851.573803432</v>
+        <v>5521921.937907781</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -808,7 +1906,7 @@
         <v>2030</v>
       </c>
       <c r="B8">
-        <v>8496392.817765646</v>
+        <v>5031790.464724424</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -816,7 +1914,7 @@
         <v>2031</v>
       </c>
       <c r="B9">
-        <v>9056455.227835827</v>
+        <v>4841199.588859485</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -824,7 +1922,7 @@
         <v>2032</v>
       </c>
       <c r="B10">
-        <v>9255619.398572583</v>
+        <v>4769247.993966782</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -832,7 +1930,7 @@
         <v>2033</v>
       </c>
       <c r="B11">
-        <v>9904333.984707642</v>
+        <v>4828123.562742811</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -840,7 +1938,7 @@
         <v>2034</v>
       </c>
       <c r="B12">
-        <v>8840679.935987633</v>
+        <v>4513117.161228755</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -848,7 +1946,7 @@
         <v>2035</v>
       </c>
       <c r="B13">
-        <v>9388959.156573191</v>
+        <v>4468076.141771164</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -856,7 +1954,7 @@
         <v>2036</v>
       </c>
       <c r="B14">
-        <v>10083511.84565322</v>
+        <v>4803247.499205148</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -864,7 +1962,7 @@
         <v>2037</v>
       </c>
       <c r="B15">
-        <v>8980054.468417412</v>
+        <v>3331335.740500649</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -872,7 +1970,7 @@
         <v>2038</v>
       </c>
       <c r="B16">
-        <v>9808145.172027892</v>
+        <v>3610502.407590034</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -880,7 +1978,7 @@
         <v>2039</v>
       </c>
       <c r="B17">
-        <v>10832623.48181518</v>
+        <v>3958685.510956987</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -888,7 +1986,7 @@
         <v>2040</v>
       </c>
       <c r="B18">
-        <v>11351116.19753434</v>
+        <v>3718867.835375945</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -896,7 +1994,7 @@
         <v>2041</v>
       </c>
       <c r="B19">
-        <v>11569728.63170497</v>
+        <v>4159074.371942916</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -904,7 +2002,7 @@
         <v>2042</v>
       </c>
       <c r="B20">
-        <v>12026256.87803554</v>
+        <v>4395593.908635538</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -912,7 +2010,1093 @@
         <v>2043</v>
       </c>
       <c r="B21">
-        <v>12390830.27578433</v>
+        <v>4383315.791971725</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>2024</v>
+      </c>
+      <c r="B2">
+        <v>6656365.637446346</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>2025</v>
+      </c>
+      <c r="B3">
+        <v>5619770.708313709</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>2026</v>
+      </c>
+      <c r="B4">
+        <v>6812938.332080998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>2027</v>
+      </c>
+      <c r="B5">
+        <v>6809999.237246415</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>2028</v>
+      </c>
+      <c r="B6">
+        <v>6830497.440366244</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>2029</v>
+      </c>
+      <c r="B7">
+        <v>6425516.595092738</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>2030</v>
+      </c>
+      <c r="B8">
+        <v>5075086.366980183</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <v>2031</v>
+      </c>
+      <c r="B9">
+        <v>5019799.564332146</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>2032</v>
+      </c>
+      <c r="B10">
+        <v>4956259.9581774</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11">
+        <v>2033</v>
+      </c>
+      <c r="B11">
+        <v>5439862.245418669</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12">
+        <v>2034</v>
+      </c>
+      <c r="B12">
+        <v>4569758.823525483</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13">
+        <v>2035</v>
+      </c>
+      <c r="B13">
+        <v>4189526.231131611</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14">
+        <v>2036</v>
+      </c>
+      <c r="B14">
+        <v>4612378.420465598</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15">
+        <v>2037</v>
+      </c>
+      <c r="B15">
+        <v>4159055.071314048</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16">
+        <v>2038</v>
+      </c>
+      <c r="B16">
+        <v>4720650.735717795</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17">
+        <v>2039</v>
+      </c>
+      <c r="B17">
+        <v>5200602.00918534</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18">
+        <v>2040</v>
+      </c>
+      <c r="B18">
+        <v>5458527.703828252</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19">
+        <v>2041</v>
+      </c>
+      <c r="B19">
+        <v>5777676.479133485</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20">
+        <v>2042</v>
+      </c>
+      <c r="B20">
+        <v>6293417.772231379</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21">
+        <v>2043</v>
+      </c>
+      <c r="B21">
+        <v>6577012.387612106</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>2024</v>
+      </c>
+      <c r="B2">
+        <v>3951910.888327728</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>2025</v>
+      </c>
+      <c r="B3">
+        <v>3896760.304140996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>2026</v>
+      </c>
+      <c r="B4">
+        <v>4546436.307480475</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>2027</v>
+      </c>
+      <c r="B5">
+        <v>4955967.997034571</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>2028</v>
+      </c>
+      <c r="B6">
+        <v>5111097.587182011</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>2029</v>
+      </c>
+      <c r="B7">
+        <v>5266145.212657541</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>2030</v>
+      </c>
+      <c r="B8">
+        <v>5017519.322896725</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <v>2031</v>
+      </c>
+      <c r="B9">
+        <v>4574874.429431391</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>2032</v>
+      </c>
+      <c r="B10">
+        <v>4455885.522870324</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11">
+        <v>2033</v>
+      </c>
+      <c r="B11">
+        <v>4527288.956628951</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12">
+        <v>2034</v>
+      </c>
+      <c r="B12">
+        <v>3938478.580466065</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13">
+        <v>2035</v>
+      </c>
+      <c r="B13">
+        <v>3441750.39992673</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14">
+        <v>2036</v>
+      </c>
+      <c r="B14">
+        <v>3693579.873799298</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15">
+        <v>2037</v>
+      </c>
+      <c r="B15">
+        <v>3203478.764278796</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16">
+        <v>2038</v>
+      </c>
+      <c r="B16">
+        <v>3216256.961531587</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17">
+        <v>2039</v>
+      </c>
+      <c r="B17">
+        <v>3544095.344050987</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18">
+        <v>2040</v>
+      </c>
+      <c r="B18">
+        <v>3506767.849314635</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19">
+        <v>2041</v>
+      </c>
+      <c r="B19">
+        <v>3985156.031115565</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20">
+        <v>2042</v>
+      </c>
+      <c r="B20">
+        <v>4042051.930917169</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21">
+        <v>2043</v>
+      </c>
+      <c r="B21">
+        <v>4236864.523604972</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>2024</v>
+      </c>
+      <c r="B2">
+        <v>7499026.829941634</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>2025</v>
+      </c>
+      <c r="B3">
+        <v>6282243.878390167</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>2026</v>
+      </c>
+      <c r="B4">
+        <v>7413402.299742431</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>2027</v>
+      </c>
+      <c r="B5">
+        <v>8078012.344860101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>2028</v>
+      </c>
+      <c r="B6">
+        <v>8152425.86897608</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>2029</v>
+      </c>
+      <c r="B7">
+        <v>8400661.871458042</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>2030</v>
+      </c>
+      <c r="B8">
+        <v>8207821.343610279</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <v>2031</v>
+      </c>
+      <c r="B9">
+        <v>8751324.446800245</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>2032</v>
+      </c>
+      <c r="B10">
+        <v>8939568.85699724</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11">
+        <v>2033</v>
+      </c>
+      <c r="B11">
+        <v>9567627.857173232</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12">
+        <v>2034</v>
+      </c>
+      <c r="B12">
+        <v>8543549.69235404</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13">
+        <v>2035</v>
+      </c>
+      <c r="B13">
+        <v>9070246.894371806</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14">
+        <v>2036</v>
+      </c>
+      <c r="B14">
+        <v>9735464.336171718</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15">
+        <v>2037</v>
+      </c>
+      <c r="B15">
+        <v>8672967.028321913</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16">
+        <v>2038</v>
+      </c>
+      <c r="B16">
+        <v>9467767.032271439</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17">
+        <v>2039</v>
+      </c>
+      <c r="B17">
+        <v>10450475.12074826</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18">
+        <v>2040</v>
+      </c>
+      <c r="B18">
+        <v>10946648.87480488</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19">
+        <v>2041</v>
+      </c>
+      <c r="B19">
+        <v>11158353.21086289</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20">
+        <v>2042</v>
+      </c>
+      <c r="B20">
+        <v>11599259.03731799</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21">
+        <v>2043</v>
+      </c>
+      <c r="B21">
+        <v>11948646.3913637</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>2024</v>
+      </c>
+      <c r="B2">
+        <v>4637828.334188421</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>2025</v>
+      </c>
+      <c r="B3">
+        <v>4709979.870176958</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>2026</v>
+      </c>
+      <c r="B4">
+        <v>5565515.590248153</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>2027</v>
+      </c>
+      <c r="B5">
+        <v>6052384.325216115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>2028</v>
+      </c>
+      <c r="B6">
+        <v>6215234.366004166</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>2029</v>
+      </c>
+      <c r="B7">
+        <v>6620315.36499203</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>2030</v>
+      </c>
+      <c r="B8">
+        <v>6457280.223308306</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <v>2031</v>
+      </c>
+      <c r="B9">
+        <v>6557625.26830286</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>2032</v>
+      </c>
+      <c r="B10">
+        <v>6637674.852401175</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11">
+        <v>2033</v>
+      </c>
+      <c r="B11">
+        <v>6834107.431569878</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12">
+        <v>2034</v>
+      </c>
+      <c r="B12">
+        <v>6651809.859250412</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13">
+        <v>2035</v>
+      </c>
+      <c r="B13">
+        <v>6148288.334643951</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14">
+        <v>2036</v>
+      </c>
+      <c r="B14">
+        <v>6470540.090835414</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15">
+        <v>2037</v>
+      </c>
+      <c r="B15">
+        <v>6227163.465751998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16">
+        <v>2038</v>
+      </c>
+      <c r="B16">
+        <v>6846871.985410713</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17">
+        <v>2039</v>
+      </c>
+      <c r="B17">
+        <v>7596771.273097109</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18">
+        <v>2040</v>
+      </c>
+      <c r="B18">
+        <v>8073453.196467299</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19">
+        <v>2041</v>
+      </c>
+      <c r="B19">
+        <v>8230078.927408461</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20">
+        <v>2042</v>
+      </c>
+      <c r="B20">
+        <v>8351939.515715674</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21">
+        <v>2043</v>
+      </c>
+      <c r="B21">
+        <v>8592774.189751953</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>2024</v>
+      </c>
+      <c r="B2">
+        <v>5144671.292886975</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>2025</v>
+      </c>
+      <c r="B3">
+        <v>5327735.24908313</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>2026</v>
+      </c>
+      <c r="B4">
+        <v>6265413.683936646</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>2027</v>
+      </c>
+      <c r="B5">
+        <v>6679755.444784267</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>2028</v>
+      </c>
+      <c r="B6">
+        <v>6619514.287566469</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>2029</v>
+      </c>
+      <c r="B7">
+        <v>7238106.858845249</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>2030</v>
+      </c>
+      <c r="B8">
+        <v>6614011.598527758</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <v>2031</v>
+      </c>
+      <c r="B9">
+        <v>6370646.939114903</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>2032</v>
+      </c>
+      <c r="B10">
+        <v>6285710.112507201</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11">
+        <v>2033</v>
+      </c>
+      <c r="B11">
+        <v>6362415.552675538</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12">
+        <v>2034</v>
+      </c>
+      <c r="B12">
+        <v>5954543.246707993</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13">
+        <v>2035</v>
+      </c>
+      <c r="B13">
+        <v>5896986.127254719</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14">
+        <v>2036</v>
+      </c>
+      <c r="B14">
+        <v>6338223.303712519</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15">
+        <v>2037</v>
+      </c>
+      <c r="B15">
+        <v>4413533.207928475</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16">
+        <v>2038</v>
+      </c>
+      <c r="B16">
+        <v>4780424.972319666</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17">
+        <v>2039</v>
+      </c>
+      <c r="B17">
+        <v>5232168.315327813</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18">
+        <v>2040</v>
+      </c>
+      <c r="B18">
+        <v>4917948.444624167</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19">
+        <v>2041</v>
+      </c>
+      <c r="B19">
+        <v>5490063.60883139</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20">
+        <v>2042</v>
+      </c>
+      <c r="B20">
+        <v>5801321.871104096</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21">
+        <v>2043</v>
+      </c>
+      <c r="B21">
+        <v>5777101.076326042</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>2024</v>
+      </c>
+      <c r="B2">
+        <v>8718287.855083594</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>2025</v>
+      </c>
+      <c r="B3">
+        <v>7364166.977131634</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>2026</v>
+      </c>
+      <c r="B4">
+        <v>8921196.550037829</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>2027</v>
+      </c>
+      <c r="B5">
+        <v>8926006.398923881</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>2028</v>
+      </c>
+      <c r="B6">
+        <v>8948918.153986501</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>2029</v>
+      </c>
+      <c r="B7">
+        <v>8434635.876146475</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>2030</v>
+      </c>
+      <c r="B8">
+        <v>6685019.012075348</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <v>2031</v>
+      </c>
+      <c r="B9">
+        <v>6608478.622179671</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>2032</v>
+      </c>
+      <c r="B10">
+        <v>6530862.075616133</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11">
+        <v>2033</v>
+      </c>
+      <c r="B11">
+        <v>7165650.117206151</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12">
+        <v>2034</v>
+      </c>
+      <c r="B12">
+        <v>6025609.171675636</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13">
+        <v>2035</v>
+      </c>
+      <c r="B13">
+        <v>5529626.936916162</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14">
+        <v>2036</v>
+      </c>
+      <c r="B14">
+        <v>6079757.365401715</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15">
+        <v>2037</v>
+      </c>
+      <c r="B15">
+        <v>5486975.051469157</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16">
+        <v>2038</v>
+      </c>
+      <c r="B16">
+        <v>6217148.388190486</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17">
+        <v>2039</v>
+      </c>
+      <c r="B17">
+        <v>6845937.235418542</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18">
+        <v>2040</v>
+      </c>
+      <c r="B18">
+        <v>7190299.645281721</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19">
+        <v>2041</v>
+      </c>
+      <c r="B19">
+        <v>7606167.714074999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20">
+        <v>2042</v>
+      </c>
+      <c r="B20">
+        <v>8280388.356627382</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21">
+        <v>2043</v>
+      </c>
+      <c r="B21">
+        <v>8650367.774567269</v>
       </c>
     </row>
   </sheetData>

</xml_diff>